<commit_message>
Correcciones Cargas Masivas, Validaciones y Numerar Facturas
</commit_message>
<xml_diff>
--- a/LQCE/LQCE.SharePoint/Layouts/Prestaciones/PrestacionesHumanas.xlsx
+++ b/LQCE/LQCE.SharePoint/Layouts/Prestaciones/PrestacionesHumanas.xlsx
@@ -447,20 +447,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>

</xml_diff>